<commit_message>
Latest changes with documentation
</commit_message>
<xml_diff>
--- a/03_time_report/Hours worked 15 Nov - 30 Sept 2025.xlsx
+++ b/03_time_report/Hours worked 15 Nov - 30 Sept 2025.xlsx
@@ -55,7 +55,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -78,30 +78,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -425,7 +413,7 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -461,15 +449,15 @@
         <v>15.75</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:C7" si="0">(C3-B4)</f>
+        <f t="shared" ref="C4:C8" si="0">(C3-B4)</f>
         <v>102.85</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="4">
-        <f>SUM(B2:B7)</f>
-        <v>119.25</v>
+      <c r="H4" s="3">
+        <f>SUM(B2:B8)</f>
+        <v>120.75</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -491,21 +479,33 @@
       <c r="B6" s="1">
         <v>51.5</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="4">
         <f t="shared" si="0"/>
         <v>31.849999999999994</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>6.2024999999999997</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>12.5</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="4">
         <f t="shared" si="0"/>
         <v>19.349999999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4">
+        <v>7.2024999999999997</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>17.849999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code fixed and report updated
</commit_message>
<xml_diff>
--- a/03_time_report/Hours worked 15 Nov - 30 Sept 2025.xlsx
+++ b/03_time_report/Hours worked 15 Nov - 30 Sept 2025.xlsx
@@ -55,7 +55,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -78,11 +78,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -90,6 +101,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -449,15 +461,15 @@
         <v>15.75</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:C8" si="0">(C3-B4)</f>
+        <f t="shared" ref="C4:C9" si="0">(C3-B4)</f>
         <v>102.85</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="3">
-        <f>SUM(B2:B8)</f>
-        <v>120.75</v>
+        <f>SUM(B2:B9)</f>
+        <v>122.75</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -506,6 +518,18 @@
       <c r="C8" s="4">
         <f t="shared" si="0"/>
         <v>17.849999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="5">
+        <v>8.2025000000000006</v>
+      </c>
+      <c r="B9" s="5">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>15.849999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>